<commit_message>
adding last half of recorded selectors to excel inputs
</commit_message>
<xml_diff>
--- a/random_value_generator.xlsx
+++ b/random_value_generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Senthil\Documents\UiPath\RandomFill_CMS1500\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F710FAB5-5EE8-4D95-9F53-9CC9588BE8A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9565C9-A170-4D37-B0C7-820E520B0BD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25490" yWindow="1510" windowWidth="19420" windowHeight="10420" xr2:uid="{A1A1DBE5-A83A-4576-8996-061BE4D33211}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="96">
   <si>
     <t>1. Medicare</t>
   </si>
@@ -305,6 +305,45 @@
   </si>
   <si>
     <t>14. Illness QUAL</t>
+  </si>
+  <si>
+    <t>24.1.B Place of Service</t>
+  </si>
+  <si>
+    <t>24.2.A from MM</t>
+  </si>
+  <si>
+    <t>24.2.A from DD</t>
+  </si>
+  <si>
+    <t>24.2.A from YY</t>
+  </si>
+  <si>
+    <t>24.2.A to MM</t>
+  </si>
+  <si>
+    <t>24.2.A to DD</t>
+  </si>
+  <si>
+    <t>24.2.A to YY</t>
+  </si>
+  <si>
+    <t>24.2.B Place of Service</t>
+  </si>
+  <si>
+    <t>24.2.D CPT/MCPCS</t>
+  </si>
+  <si>
+    <t>24.2.E Diagnosis</t>
+  </si>
+  <si>
+    <t>24.2.F Charges</t>
+  </si>
+  <si>
+    <t>24.2.G Units</t>
+  </si>
+  <si>
+    <t>24.2.J Provider ID#</t>
   </si>
 </sst>
 </file>
@@ -674,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE2F2E9-4B7C-48F5-9711-3150F9D0912C}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59:E59"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,7 +770,7 @@
       </c>
       <c r="E3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>EiLb3226</v>
+        <v>CuLo3914</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -754,7 +793,7 @@
       </c>
       <c r="E5" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -766,7 +805,7 @@
       </c>
       <c r="E6" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -778,7 +817,7 @@
       </c>
       <c r="E7" s="4">
         <f ca="1">RANDBETWEEN(1980,2020)</f>
-        <v>2000</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -787,18 +826,18 @@
       </c>
       <c r="B8" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B8" ca="1">_xlfn.IFS(E8=1,"M",E8=2,"F")</f>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="C8" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">_xlfn.IFS(E8=1,"1",E8=2,"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="D8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="4">
         <f ca="1">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -844,7 +883,7 @@
       </c>
       <c r="E12" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>KY</v>
+        <v>PO</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -856,7 +895,7 @@
       </c>
       <c r="E13" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>55075</v>
+        <v>28715</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -868,7 +907,7 @@
       </c>
       <c r="E14" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>863</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -880,7 +919,7 @@
       </c>
       <c r="E15" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>7692596</v>
+        <v>4861621</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -889,18 +928,18 @@
       </c>
       <c r="B16" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B16" ca="1">_xlfn.IFS(E16=1,"S",E16=2,"M",E16=3,"C",E16=4,"O")</f>
-        <v>C</v>
+        <v>M</v>
       </c>
       <c r="C16" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="C16" ca="1">_xlfn.IFS(E16=1,"",E16=2,"2",E16=3,"",E16=4,"")</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="3">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -934,7 +973,7 @@
       </c>
       <c r="E19" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>CL</v>
+        <v>FX</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -946,7 +985,7 @@
       </c>
       <c r="E20" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>60482</v>
+        <v>04203</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -958,7 +997,7 @@
       </c>
       <c r="E21" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>049</v>
+        <v>956</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -970,7 +1009,7 @@
       </c>
       <c r="E22" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>3299996</v>
+        <v>7223090</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -982,7 +1021,7 @@
       </c>
       <c r="E23" s="3" t="str">
         <f ca="1">"RESERVED "&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>RESERVED ZhJs4563</v>
+        <v>RESERVED TmYj2070</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1006,7 +1045,7 @@
       </c>
       <c r="E25" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>WdJz9456</v>
+        <v>YyAx8453</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1035,18 +1074,18 @@
       </c>
       <c r="B27" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B27" ca="1">_xlfn.IFS(E27=1,"YES",E27=2,"NO")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="C27" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="C27" ca="1">_xlfn.IFS(B27="YES","5",B27="NO","1")</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="4">
         <f ca="1">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1058,7 +1097,7 @@
       </c>
       <c r="E28" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>NG</v>
+        <v>YE</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1067,18 +1106,18 @@
       </c>
       <c r="B29" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B29" ca="1">_xlfn.IFS(E29=1,"YES",E29=2,"NO")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="C29" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="C29" ca="1">_xlfn.IFS(B29="YES","4",B29="NO","2")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E29" s="4">
         <f ca="1">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1090,7 +1129,7 @@
       </c>
       <c r="E30" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>873807</v>
+        <v>945520</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1102,7 +1141,7 @@
       </c>
       <c r="E31" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>SvWz2214</v>
+        <v>ZpPp6720</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1114,7 +1153,7 @@
       </c>
       <c r="E32" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1126,7 +1165,7 @@
       </c>
       <c r="E33" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1138,7 +1177,7 @@
       </c>
       <c r="E34" s="4">
         <f ca="1">RANDBETWEEN(1980,2020)</f>
-        <v>1993</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1166,7 +1205,7 @@
       </c>
       <c r="E36" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>OaSb7985</v>
+        <v>TcVm7936</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1178,7 +1217,7 @@
       </c>
       <c r="E37" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>WnZy3660</v>
+        <v>OvMm3917</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1205,105 +1244,141 @@
       <c r="A39" t="s">
         <v>46</v>
       </c>
+      <c r="C39" s="3">
+        <v>217</v>
+      </c>
       <c r="E39" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>47</v>
       </c>
+      <c r="C40" s="3">
+        <v>218</v>
+      </c>
       <c r="E40" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>48</v>
       </c>
+      <c r="C41" s="3">
+        <v>219</v>
+      </c>
       <c r="E41" s="4">
         <f ca="1">RANDBETWEEN(1980,2020)</f>
-        <v>1995</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>82</v>
       </c>
+      <c r="C42" s="3">
+        <v>216</v>
+      </c>
       <c r="E42" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>931</v>
+        <v>859</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>49</v>
       </c>
+      <c r="C43" s="3">
+        <v>215</v>
+      </c>
       <c r="E43" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>594</v>
+        <v>910</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>50</v>
       </c>
+      <c r="C44" s="3">
+        <v>212</v>
+      </c>
       <c r="E44" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>51</v>
       </c>
+      <c r="C45" s="3">
+        <v>213</v>
+      </c>
       <c r="E45" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>52</v>
       </c>
+      <c r="C46" s="3">
+        <v>214</v>
+      </c>
       <c r="E46" s="4">
         <f ca="1">RANDBETWEEN(1980,2020)</f>
-        <v>2012</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>53</v>
       </c>
+      <c r="C47" s="3">
+        <v>209</v>
+      </c>
       <c r="E47" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>54</v>
       </c>
+      <c r="C48" s="3">
+        <v>210</v>
+      </c>
       <c r="E48" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>55</v>
       </c>
+      <c r="C49" s="3">
+        <v>211</v>
+      </c>
       <c r="E49" s="4">
         <f ca="1">RANDBETWEEN(1980,2020)</f>
-        <v>2008</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>56</v>
       </c>
+      <c r="C50" s="3">
+        <v>21</v>
+      </c>
       <c r="E50" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
         <v>1</v>
@@ -1313,72 +1388,96 @@
       <c r="A51" t="s">
         <v>57</v>
       </c>
+      <c r="C51" s="3">
+        <v>207</v>
+      </c>
       <c r="E51" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>58</v>
       </c>
+      <c r="C52" s="3">
+        <v>208</v>
+      </c>
       <c r="E52" s="4">
         <f ca="1">RANDBETWEEN(1980,2020)</f>
-        <v>1981</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>59</v>
       </c>
+      <c r="C53" s="3">
+        <v>205</v>
+      </c>
       <c r="E53" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>60</v>
       </c>
+      <c r="C54" s="3">
+        <v>204</v>
+      </c>
       <c r="E54" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>61</v>
       </c>
+      <c r="C55" s="3">
+        <v>203</v>
+      </c>
       <c r="E55" s="4">
         <f ca="1">RANDBETWEEN(1980,2020)</f>
-        <v>1996</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>62</v>
       </c>
+      <c r="C56" s="3">
+        <v>202</v>
+      </c>
       <c r="E56" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>63</v>
       </c>
+      <c r="C57" s="3">
+        <v>201</v>
+      </c>
       <c r="E57" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>64</v>
       </c>
+      <c r="C58" s="3">
+        <v>26</v>
+      </c>
       <c r="E58" s="4">
         <f ca="1">RANDBETWEEN(1980,2020)</f>
-        <v>2000</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1387,162 +1486,378 @@
       </c>
       <c r="B59" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B59" ca="1">_xlfn.IFS(E59=1,"YES",E59=2,"NO")</f>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="C59" s="3" t="str" cm="1">
-        <f t="array" aca="1" ref="C59" ca="1">_xlfn.IFS(B59="YES","1",B59="NO","3")</f>
-        <v>3</v>
+        <f t="array" aca="1" ref="C59" ca="1">_xlfn.IFS(B59="YES","2",B59="NO","4")</f>
+        <v>2</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E59" s="4">
         <f ca="1">RANDBETWEEN(1,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>66</v>
       </c>
+      <c r="C60" s="3">
+        <v>27</v>
+      </c>
       <c r="E60" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;"."&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>643.44</v>
+        <v>684.68</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>67</v>
       </c>
+      <c r="C61" s="3">
+        <v>199</v>
+      </c>
       <c r="E61" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>0351</v>
+        <v>8945</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>68</v>
       </c>
+      <c r="C62" s="3">
+        <v>198</v>
+      </c>
       <c r="E62" s="3" t="str">
         <f t="shared" ref="E62:E64" ca="1" si="0">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>7604</v>
+        <v>3788</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>69</v>
       </c>
+      <c r="C63" s="3">
+        <v>197</v>
+      </c>
       <c r="E63" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>7671</v>
+        <v>5074</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>70</v>
       </c>
+      <c r="C64" s="3">
+        <v>196</v>
+      </c>
       <c r="E64" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>9628</v>
+        <v>5378</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>71</v>
       </c>
+      <c r="C65" s="3">
+        <v>188</v>
+      </c>
       <c r="E65" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>72</v>
       </c>
+      <c r="C66" s="3">
+        <v>187</v>
+      </c>
       <c r="E66" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>73</v>
       </c>
+      <c r="C67" s="3">
+        <v>186</v>
+      </c>
       <c r="E67" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>94</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>74</v>
       </c>
+      <c r="C68" s="3">
+        <v>185</v>
+      </c>
       <c r="E68" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>75</v>
       </c>
+      <c r="C69" s="3">
+        <v>184</v>
+      </c>
       <c r="E69" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>76</v>
       </c>
+      <c r="C70" s="3">
+        <v>183</v>
+      </c>
       <c r="E70" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>84</v>
+        <v>06</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+      <c r="C71" s="3">
+        <v>182</v>
       </c>
       <c r="E71" s="3" t="str">
-        <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>72281</v>
+        <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>77</v>
+      </c>
+      <c r="C72" s="3">
+        <v>180</v>
+      </c>
+      <c r="E72" s="3" t="str">
+        <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
+        <v>35253</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>78</v>
       </c>
-      <c r="E72" s="3" t="str">
+      <c r="C73" s="3">
+        <v>175</v>
+      </c>
+      <c r="E73" s="3" t="str">
+        <f ca="1">CHAR(RANDBETWEEN(65,90))</f>
+        <v>P</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>79</v>
+      </c>
+      <c r="C74" s="3">
+        <v>174</v>
+      </c>
+      <c r="E74" s="3" t="str">
+        <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;"."&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
+        <v>114.35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>80</v>
+      </c>
+      <c r="C75" s="3">
+        <v>172</v>
+      </c>
+      <c r="E75" s="4">
+        <f ca="1">RANDBETWEEN(0,9)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>81</v>
+      </c>
+      <c r="C76" s="3">
+        <v>39</v>
+      </c>
+      <c r="E76" s="3" t="str">
+        <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
+        <v>3628059</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>84</v>
+      </c>
+      <c r="C77" s="3">
+        <f>C65-19</f>
+        <v>169</v>
+      </c>
+      <c r="E77" s="4">
+        <f ca="1">RANDBETWEEN(1,12)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>85</v>
+      </c>
+      <c r="C78" s="3">
+        <f t="shared" ref="C78:C88" si="1">C66-19</f>
+        <v>168</v>
+      </c>
+      <c r="E78" s="4">
+        <f ca="1">RANDBETWEEN(1,31)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>86</v>
+      </c>
+      <c r="C79" s="3">
+        <f t="shared" si="1"/>
+        <v>167</v>
+      </c>
+      <c r="E79" s="3" t="str">
+        <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
+        <v>07</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>87</v>
+      </c>
+      <c r="C80" s="3">
+        <f t="shared" si="1"/>
+        <v>166</v>
+      </c>
+      <c r="E80" s="4">
+        <f ca="1">RANDBETWEEN(1,12)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>88</v>
+      </c>
+      <c r="C81" s="3">
+        <f t="shared" si="1"/>
+        <v>165</v>
+      </c>
+      <c r="E81" s="4">
+        <f ca="1">RANDBETWEEN(1,31)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>89</v>
+      </c>
+      <c r="C82" s="3">
+        <f t="shared" si="1"/>
+        <v>164</v>
+      </c>
+      <c r="E82" s="3" t="str">
+        <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>90</v>
+      </c>
+      <c r="C83" s="3">
+        <f t="shared" si="1"/>
+        <v>163</v>
+      </c>
+      <c r="E83" s="3" t="str">
+        <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>91</v>
+      </c>
+      <c r="C84" s="3">
+        <f t="shared" si="1"/>
+        <v>161</v>
+      </c>
+      <c r="E84" s="3" t="str">
+        <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
+        <v>19219</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>92</v>
+      </c>
+      <c r="C85" s="3">
+        <f t="shared" si="1"/>
+        <v>156</v>
+      </c>
+      <c r="E85" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))</f>
         <v>Q</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>79</v>
-      </c>
-      <c r="E73" s="3" t="str">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>93</v>
+      </c>
+      <c r="C86" s="3">
+        <f t="shared" si="1"/>
+        <v>155</v>
+      </c>
+      <c r="E86" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;"."&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>255.35</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>80</v>
-      </c>
-      <c r="E74" s="4">
+        <v>952.75</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>94</v>
+      </c>
+      <c r="C87" s="3">
+        <f t="shared" si="1"/>
+        <v>153</v>
+      </c>
+      <c r="E87" s="4">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>81</v>
-      </c>
-      <c r="E75" s="3" t="str">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>95</v>
+      </c>
+      <c r="C88" s="3">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="E88" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>4506610</v>
+        <v>2770115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing error with selecting pdf elements on startup
</commit_message>
<xml_diff>
--- a/random_value_generator.xlsx
+++ b/random_value_generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Senthil\Documents\UiPath\RandomFill_CMS1500\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9565C9-A170-4D37-B0C7-820E520B0BD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C46E083-32F9-410B-A66F-4701B413354F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25490" yWindow="1510" windowWidth="19420" windowHeight="10420" xr2:uid="{A1A1DBE5-A83A-4576-8996-061BE4D33211}"/>
   </bookViews>
@@ -715,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE2F2E9-4B7C-48F5-9711-3150F9D0912C}">
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,14 +751,14 @@
       </c>
       <c r="B2" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">_xlfn.IFS(E2=1,"Medicare",E2=2,"Medicaid",E2=3,"Tricare",E2=4,"Champva",E2=5,"Group",E2=6,"Feca",E2=7,"Other")</f>
-        <v>Other</v>
+        <v>Medicare</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="3">
         <f ca="1">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -770,7 +770,7 @@
       </c>
       <c r="E3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>CuLo3914</v>
+        <v>UwJi8852</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -805,7 +805,7 @@
       </c>
       <c r="E6" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -817,7 +817,7 @@
       </c>
       <c r="E7" s="4">
         <f ca="1">RANDBETWEEN(1980,2020)</f>
-        <v>1980</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -883,7 +883,7 @@
       </c>
       <c r="E12" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>PO</v>
+        <v>DK</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -895,7 +895,7 @@
       </c>
       <c r="E13" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>28715</v>
+        <v>39743</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -907,7 +907,7 @@
       </c>
       <c r="E14" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>176</v>
+        <v>439</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -919,7 +919,7 @@
       </c>
       <c r="E15" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>4861621</v>
+        <v>4963895</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -973,7 +973,7 @@
       </c>
       <c r="E19" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>FX</v>
+        <v>VY</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -985,7 +985,7 @@
       </c>
       <c r="E20" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>04203</v>
+        <v>82600</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -997,7 +997,7 @@
       </c>
       <c r="E21" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>956</v>
+        <v>518</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1009,7 +1009,7 @@
       </c>
       <c r="E22" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>7223090</v>
+        <v>9445644</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="E23" s="3" t="str">
         <f ca="1">"RESERVED "&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>RESERVED TmYj2070</v>
+        <v>RESERVED CwHu4501</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1045,7 +1045,7 @@
       </c>
       <c r="E25" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>YyAx8453</v>
+        <v>QmSo1325</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="E28" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>YE</v>
+        <v>QE</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1129,7 +1129,7 @@
       </c>
       <c r="E30" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>945520</v>
+        <v>687340</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="E31" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>ZpPp6720</v>
+        <v>SvRj6734</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="E32" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="E33" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="E34" s="4">
         <f ca="1">RANDBETWEEN(1980,2020)</f>
-        <v>2004</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="E36" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>TcVm7936</v>
+        <v>MoWa7513</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1217,7 +1217,7 @@
       </c>
       <c r="E37" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>OvMm3917</v>
+        <v>EeVn8047</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="E39" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="E41" s="4">
         <f ca="1">RANDBETWEEN(1980,2020)</f>
-        <v>2005</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="E42" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>859</v>
+        <v>251</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="E43" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>910</v>
+        <v>907</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="E44" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="E45" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="E46" s="4">
         <f ca="1">RANDBETWEEN(1980,2020)</f>
-        <v>2020</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="E48" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1369,7 +1369,7 @@
       </c>
       <c r="E49" s="4">
         <f ca="1">RANDBETWEEN(1980,2020)</f>
-        <v>1984</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="E51" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1405,7 +1405,7 @@
       </c>
       <c r="E52" s="4">
         <f ca="1">RANDBETWEEN(1980,2020)</f>
-        <v>1982</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="E53" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1429,7 +1429,7 @@
       </c>
       <c r="E54" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="E55" s="4">
         <f ca="1">RANDBETWEEN(1980,2020)</f>
-        <v>2019</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="E57" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1477,7 +1477,7 @@
       </c>
       <c r="E58" s="4">
         <f ca="1">RANDBETWEEN(1980,2020)</f>
-        <v>1993</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1486,18 +1486,18 @@
       </c>
       <c r="B59" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="B59" ca="1">_xlfn.IFS(E59=1,"YES",E59=2,"NO")</f>
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="C59" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="C59" ca="1">_xlfn.IFS(B59="YES","2",B59="NO","4")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E59" s="4">
         <f ca="1">RANDBETWEEN(1,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -1509,7 +1509,7 @@
       </c>
       <c r="E60" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;"."&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>684.68</v>
+        <v>296.39</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="E61" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>8945</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -1533,7 +1533,7 @@
       </c>
       <c r="E62" s="3" t="str">
         <f t="shared" ref="E62:E64" ca="1" si="0">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>3788</v>
+        <v>6016</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1545,7 +1545,7 @@
       </c>
       <c r="E63" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>5074</v>
+        <v>0858</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -1557,7 +1557,7 @@
       </c>
       <c r="E64" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>5378</v>
+        <v>9567</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -1569,7 +1569,7 @@
       </c>
       <c r="E65" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="E66" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -1605,7 +1605,7 @@
       </c>
       <c r="E68" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -1617,7 +1617,7 @@
       </c>
       <c r="E69" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -1629,7 +1629,7 @@
       </c>
       <c r="E70" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>06</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="E71" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>59</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -1653,7 +1653,7 @@
       </c>
       <c r="E72" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>35253</v>
+        <v>11962</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -1665,7 +1665,7 @@
       </c>
       <c r="E73" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))</f>
-        <v>P</v>
+        <v>O</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -1677,7 +1677,7 @@
       </c>
       <c r="E74" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;"."&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>114.35</v>
+        <v>306.02</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -1701,7 +1701,7 @@
       </c>
       <c r="E76" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>3628059</v>
+        <v>4748557</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -1714,7 +1714,7 @@
       </c>
       <c r="E77" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -1727,7 +1727,7 @@
       </c>
       <c r="E78" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -1740,7 +1740,7 @@
       </c>
       <c r="E79" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>07</v>
+        <v>00</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="E80" s="4">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="E81" s="4">
         <f ca="1">RANDBETWEEN(1,31)</f>
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -1779,7 +1779,7 @@
       </c>
       <c r="E82" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>34</v>
+        <v>52</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="E83" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>67</v>
+        <v>23</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -1805,7 +1805,7 @@
       </c>
       <c r="E84" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>19219</v>
+        <v>59950</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -1818,7 +1818,7 @@
       </c>
       <c r="E85" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))</f>
-        <v>Q</v>
+        <v>O</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -1831,7 +1831,7 @@
       </c>
       <c r="E86" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;"."&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>952.75</v>
+        <v>939.67</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -1844,7 +1844,7 @@
       </c>
       <c r="E87" s="4">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
@@ -1852,12 +1852,11 @@
         <v>95</v>
       </c>
       <c r="C88" s="3">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="E88" s="3" t="str">
         <f ca="1">RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>2770115</v>
+        <v>3437265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>